<commit_message>
[#182385240] fix xlsx photometer data upload
</commit_message>
<xml_diff>
--- a/spec/fixtures/files/photometer_data.xlsx
+++ b/spec/fixtures/files/photometer_data.xlsx
@@ -8,7 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="photometer_xlsv" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="photometer_data" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -155,7 +155,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -244,42 +243,42 @@
   <dimension ref="A1:AF4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.22"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.25"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.18"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="23.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="23.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="8.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="23.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="8.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="23.98"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="8.32"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="29.44"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="45.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="10.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="7.94"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="23.27"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="22.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="17.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="22.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="17.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="22.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="17.06"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="22.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="17.06"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="8.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="17.96"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.6"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="12.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="15.61"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="24.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="24.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="14" min="14" style="0" width="24.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="15" min="15" style="0" width="8.23"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16" min="16" style="0" width="24.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="17" min="17" style="0" width="8.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="29.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="47.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="0" width="10.32"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="0" width="7.95"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="22" style="0" width="19.49"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="23" min="23" style="0" width="23.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="24" style="0" width="11.85"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="25" style="0" width="23.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="26" min="26" style="0" width="17.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="27" min="27" style="0" width="23.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="28" min="28" style="0" width="17.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="29" min="29" style="0" width="23.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="30" min="30" style="0" width="17.55"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="31" min="31" style="0" width="23.24"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="32" min="32" style="0" width="17.55"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -641,7 +640,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>